<commit_message>
added CRUD on participants
</commit_message>
<xml_diff>
--- a/public/uploads/participants.xlsx
+++ b/public/uploads/participants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\symfony-winter-contest\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C18B531-8484-4B0B-A47A-051F79AA3A11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7947DA1F-3E23-41B9-A6C6-04CB118C0420}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="495" windowWidth="22590" windowHeight="11415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="1185" windowWidth="22590" windowHeight="11415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>nom_participant</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Colmar</t>
+  </si>
+  <si>
+    <t>img.jpg</t>
+  </si>
+  <si>
+    <t>img.png</t>
   </si>
 </sst>
 </file>
@@ -404,7 +410,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,6 +445,9 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
@@ -455,6 +464,9 @@
       </c>
       <c r="C3" t="s">
         <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>14</v>

</xml_diff>